<commit_message>
TLWP-990 - fix provider name on spreadsheet
Also removed header with filters and added blank line after header
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application/Templates/ShowMeEverythingReportTemplate.xlsx
+++ b/src/Sfa.Tl.Matching.Application/Templates/ShowMeEverythingReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\esfa\tl-matching\src\Sfa.Tl.Matching.Application\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0C4EC9-F2CC-4563-969C-95FE3C25ECD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB8B309-4653-46A1-8FB8-DC4AD1461A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="-15510" windowWidth="22845" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="18224" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Provider name</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Showing providers with courses in these skill areas: </t>
   </si>
   <si>
     <t xml:space="preserve">Distance from </t>
@@ -95,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -103,10 +100,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,10 +315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -342,60 +335,42 @@
     <col min="11" max="11" width="21.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>